<commit_message>
add ETA and word file
</commit_message>
<xml_diff>
--- a/two file/excel file.xlsx
+++ b/two file/excel file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MinhHy1\Github\Le_Minh_Hy\two file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCADD6C-6E44-49BA-89DD-6CB8B8D429CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E1459C-5F40-4909-9F84-3303DAB594E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>No.</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>ETA</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,7 +371,7 @@
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,6 +383,9 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>